<commit_message>
update timelog with todays meeting
</commit_message>
<xml_diff>
--- a/Documents/Timelogs/Timelog - Marcellus.xlsx
+++ b/Documents/Timelogs/Timelog - Marcellus.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3560" yWindow="6340" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Hours</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>push changes to repository and discuss changes and group presentation</t>
+  </si>
+  <si>
+    <t>16/9/14</t>
+  </si>
+  <si>
+    <t>Combined Requirements Documents for the computer and pushed them into repository</t>
   </si>
 </sst>
 </file>
@@ -873,9 +879,15 @@
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A8" s="7"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="11"/>
+      <c r="A8" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="10">
+        <v>1</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>12</v>
+      </c>
       <c r="D8" s="4"/>
       <c r="E8" s="5"/>
     </row>

</xml_diff>